<commit_message>
Data Gathering Relevance Finder bug fixed and data refreshed with the new algorithm
</commit_message>
<xml_diff>
--- a/Second Iteration Data/data_gathered_part_first_segmentation.xlsx
+++ b/Second Iteration Data/data_gathered_part_first_segmentation.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87A2D293-16C7-4E87-B5A0-B891B56B9277}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECB7524A-3F7B-4C17-B445-9FB0806BF69A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3525" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3199" uniqueCount="172">
   <si>
     <t>tag_h</t>
   </si>
@@ -890,10 +890,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q804"/>
+  <dimension ref="A1:S804"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="T2" sqref="T2:T3"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -902,14 +902,14 @@
     <col min="5" max="5" width="9.5546875" customWidth="1"/>
     <col min="6" max="6" width="12" customWidth="1"/>
     <col min="7" max="7" width="15.6640625" customWidth="1"/>
-    <col min="8" max="8" width="18.77734375" customWidth="1"/>
+    <col min="8" max="8" width="16.44140625" customWidth="1"/>
     <col min="9" max="9" width="11.6640625" customWidth="1"/>
     <col min="10" max="10" width="12.44140625" customWidth="1"/>
     <col min="15" max="15" width="19.5546875" customWidth="1"/>
     <col min="16" max="16" width="16.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -959,7 +959,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -982,7 +982,7 @@
         <v>3.4146341463414602E-2</v>
       </c>
       <c r="H2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I2" t="s">
         <v>16</v>
@@ -1012,7 +1012,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1035,7 +1035,7 @@
         <v>9.3229227362778236E-4</v>
       </c>
       <c r="H3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I3" t="s">
         <v>16</v>
@@ -1064,8 +1064,12 @@
       <c r="Q3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="S3" t="str">
+        <f>IF(K2:K804&lt;0,K2,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1084,8 +1088,8 @@
       <c r="F4">
         <v>1</v>
       </c>
-      <c r="G4" t="s">
-        <v>19</v>
+      <c r="G4">
+        <v>1</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -1118,7 +1122,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>0</v>
       </c>
@@ -1137,8 +1141,8 @@
       <c r="F5">
         <v>1</v>
       </c>
-      <c r="G5" t="s">
-        <v>19</v>
+      <c r="G5">
+        <v>1</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -1171,7 +1175,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>1</v>
       </c>
@@ -1190,8 +1194,8 @@
       <c r="F6">
         <v>1</v>
       </c>
-      <c r="G6" t="s">
-        <v>19</v>
+      <c r="G6">
+        <v>1</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -1224,7 +1228,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>2</v>
       </c>
@@ -1247,7 +1251,7 @@
         <v>4.9331778634855144E-4</v>
       </c>
       <c r="H7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I7" t="s">
         <v>16</v>
@@ -1277,7 +1281,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>3</v>
       </c>
@@ -1330,7 +1334,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>4</v>
       </c>
@@ -1383,7 +1387,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>5</v>
       </c>
@@ -1436,7 +1440,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>6</v>
       </c>
@@ -1489,7 +1493,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>7</v>
       </c>
@@ -1542,7 +1546,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>8</v>
       </c>
@@ -1595,7 +1599,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>9</v>
       </c>
@@ -1648,7 +1652,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>10</v>
       </c>
@@ -1667,8 +1671,8 @@
       <c r="F15">
         <v>1</v>
       </c>
-      <c r="G15" t="s">
-        <v>19</v>
+      <c r="G15">
+        <v>1</v>
       </c>
       <c r="H15">
         <v>0</v>
@@ -1701,7 +1705,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>0</v>
       </c>
@@ -1989,7 +1993,7 @@
         <v>4.3876968978982933E-5</v>
       </c>
       <c r="H21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I21" t="s">
         <v>16</v>
@@ -2462,8 +2466,8 @@
       <c r="F30">
         <v>1</v>
       </c>
-      <c r="G30" t="s">
-        <v>19</v>
+      <c r="G30">
+        <v>1</v>
       </c>
       <c r="H30">
         <v>0</v>
@@ -2515,8 +2519,8 @@
       <c r="F31">
         <v>1</v>
       </c>
-      <c r="G31" t="s">
-        <v>19</v>
+      <c r="G31">
+        <v>1</v>
       </c>
       <c r="H31">
         <v>0</v>
@@ -2568,8 +2572,8 @@
       <c r="F32">
         <v>1</v>
       </c>
-      <c r="G32" t="s">
-        <v>19</v>
+      <c r="G32">
+        <v>1</v>
       </c>
       <c r="H32">
         <v>0</v>
@@ -2621,8 +2625,8 @@
       <c r="F33">
         <v>1</v>
       </c>
-      <c r="G33" t="s">
-        <v>19</v>
+      <c r="G33">
+        <v>1</v>
       </c>
       <c r="H33">
         <v>0</v>
@@ -2727,8 +2731,8 @@
       <c r="F35">
         <v>1</v>
       </c>
-      <c r="G35" t="s">
-        <v>19</v>
+      <c r="G35">
+        <v>1</v>
       </c>
       <c r="H35">
         <v>0</v>
@@ -2936,8 +2940,8 @@
       <c r="F39">
         <v>1</v>
       </c>
-      <c r="G39" t="s">
-        <v>19</v>
+      <c r="G39">
+        <v>1</v>
       </c>
       <c r="H39">
         <v>0</v>
@@ -2989,8 +2993,8 @@
       <c r="F40">
         <v>1</v>
       </c>
-      <c r="G40" t="s">
-        <v>19</v>
+      <c r="G40">
+        <v>1</v>
       </c>
       <c r="H40">
         <v>0</v>
@@ -3042,8 +3046,8 @@
       <c r="F41">
         <v>1</v>
       </c>
-      <c r="G41" t="s">
-        <v>19</v>
+      <c r="G41">
+        <v>1</v>
       </c>
       <c r="H41">
         <v>0</v>
@@ -3095,8 +3099,8 @@
       <c r="F42">
         <v>1</v>
       </c>
-      <c r="G42" t="s">
-        <v>19</v>
+      <c r="G42">
+        <v>1</v>
       </c>
       <c r="H42">
         <v>0</v>
@@ -3201,8 +3205,8 @@
       <c r="F44">
         <v>1</v>
       </c>
-      <c r="G44" t="s">
-        <v>19</v>
+      <c r="G44">
+        <v>1</v>
       </c>
       <c r="H44">
         <v>0</v>
@@ -3254,8 +3258,8 @@
       <c r="F45">
         <v>1</v>
       </c>
-      <c r="G45" t="s">
-        <v>19</v>
+      <c r="G45">
+        <v>1</v>
       </c>
       <c r="H45">
         <v>0</v>
@@ -3360,8 +3364,8 @@
       <c r="F47">
         <v>1</v>
       </c>
-      <c r="G47" t="s">
-        <v>19</v>
+      <c r="G47">
+        <v>1</v>
       </c>
       <c r="H47">
         <v>0</v>
@@ -3413,8 +3417,8 @@
       <c r="F48">
         <v>1</v>
       </c>
-      <c r="G48" t="s">
-        <v>19</v>
+      <c r="G48">
+        <v>1</v>
       </c>
       <c r="H48">
         <v>0</v>
@@ -3519,8 +3523,8 @@
       <c r="F50">
         <v>1</v>
       </c>
-      <c r="G50" t="s">
-        <v>19</v>
+      <c r="G50">
+        <v>1</v>
       </c>
       <c r="H50">
         <v>0</v>
@@ -3572,8 +3576,8 @@
       <c r="F51">
         <v>1</v>
       </c>
-      <c r="G51" t="s">
-        <v>19</v>
+      <c r="G51">
+        <v>1</v>
       </c>
       <c r="H51">
         <v>0</v>
@@ -3625,8 +3629,8 @@
       <c r="F52">
         <v>1</v>
       </c>
-      <c r="G52" t="s">
-        <v>19</v>
+      <c r="G52">
+        <v>1</v>
       </c>
       <c r="H52">
         <v>0</v>
@@ -3678,8 +3682,8 @@
       <c r="F53">
         <v>1</v>
       </c>
-      <c r="G53" t="s">
-        <v>19</v>
+      <c r="G53">
+        <v>1</v>
       </c>
       <c r="H53">
         <v>0</v>
@@ -3731,8 +3735,8 @@
       <c r="F54">
         <v>1</v>
       </c>
-      <c r="G54" t="s">
-        <v>19</v>
+      <c r="G54">
+        <v>1</v>
       </c>
       <c r="H54">
         <v>0</v>
@@ -3784,8 +3788,8 @@
       <c r="F55">
         <v>1</v>
       </c>
-      <c r="G55" t="s">
-        <v>19</v>
+      <c r="G55">
+        <v>1</v>
       </c>
       <c r="H55">
         <v>0</v>
@@ -4049,8 +4053,8 @@
       <c r="F60">
         <v>1</v>
       </c>
-      <c r="G60" t="s">
-        <v>19</v>
+      <c r="G60">
+        <v>1</v>
       </c>
       <c r="H60">
         <v>0</v>
@@ -4212,7 +4216,7 @@
         <v>2.949231093322098E-3</v>
       </c>
       <c r="H63">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I63" t="s">
         <v>16</v>
@@ -5041,8 +5045,8 @@
       <c r="F79">
         <v>1</v>
       </c>
-      <c r="G79" t="s">
-        <v>19</v>
+      <c r="G79">
+        <v>1</v>
       </c>
       <c r="H79">
         <v>0</v>
@@ -5094,8 +5098,8 @@
       <c r="F80">
         <v>1</v>
       </c>
-      <c r="G80" t="s">
-        <v>19</v>
+      <c r="G80">
+        <v>1</v>
       </c>
       <c r="H80">
         <v>0</v>
@@ -5253,8 +5257,8 @@
       <c r="F83">
         <v>1</v>
       </c>
-      <c r="G83" t="s">
-        <v>19</v>
+      <c r="G83">
+        <v>1</v>
       </c>
       <c r="H83">
         <v>0</v>
@@ -5306,8 +5310,8 @@
       <c r="F84">
         <v>1</v>
       </c>
-      <c r="G84" t="s">
-        <v>19</v>
+      <c r="G84">
+        <v>1</v>
       </c>
       <c r="H84">
         <v>0</v>
@@ -5359,8 +5363,8 @@
       <c r="F85">
         <v>1</v>
       </c>
-      <c r="G85" t="s">
-        <v>19</v>
+      <c r="G85">
+        <v>1</v>
       </c>
       <c r="H85">
         <v>0</v>
@@ -5412,8 +5416,8 @@
       <c r="F86">
         <v>1</v>
       </c>
-      <c r="G86" t="s">
-        <v>19</v>
+      <c r="G86">
+        <v>1</v>
       </c>
       <c r="H86">
         <v>0</v>
@@ -5889,8 +5893,8 @@
       <c r="F95">
         <v>1</v>
       </c>
-      <c r="G95" t="s">
-        <v>19</v>
+      <c r="G95">
+        <v>1</v>
       </c>
       <c r="H95">
         <v>0</v>
@@ -5942,8 +5946,8 @@
       <c r="F96">
         <v>1</v>
       </c>
-      <c r="G96" t="s">
-        <v>19</v>
+      <c r="G96">
+        <v>1</v>
       </c>
       <c r="H96">
         <v>0</v>
@@ -5995,8 +5999,8 @@
       <c r="F97">
         <v>1</v>
       </c>
-      <c r="G97" t="s">
-        <v>19</v>
+      <c r="G97">
+        <v>1</v>
       </c>
       <c r="H97">
         <v>0</v>
@@ -6101,8 +6105,8 @@
       <c r="F99">
         <v>1</v>
       </c>
-      <c r="G99" t="s">
-        <v>19</v>
+      <c r="G99">
+        <v>1</v>
       </c>
       <c r="H99">
         <v>0</v>
@@ -6582,7 +6586,7 @@
         <v>6.406149903907751E-4</v>
       </c>
       <c r="H108">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I108" t="s">
         <v>16</v>
@@ -6737,8 +6741,8 @@
       <c r="F111">
         <v>1</v>
       </c>
-      <c r="G111" t="s">
-        <v>19</v>
+      <c r="G111">
+        <v>1</v>
       </c>
       <c r="H111">
         <v>0</v>
@@ -7108,8 +7112,8 @@
       <c r="F118">
         <v>1</v>
       </c>
-      <c r="G118" t="s">
-        <v>19</v>
+      <c r="G118">
+        <v>1</v>
       </c>
       <c r="H118">
         <v>0</v>
@@ -7161,8 +7165,8 @@
       <c r="F119">
         <v>1</v>
       </c>
-      <c r="G119" t="s">
-        <v>19</v>
+      <c r="G119">
+        <v>1</v>
       </c>
       <c r="H119">
         <v>0</v>
@@ -7320,8 +7324,8 @@
       <c r="F122">
         <v>1</v>
       </c>
-      <c r="G122" t="s">
-        <v>19</v>
+      <c r="G122">
+        <v>1</v>
       </c>
       <c r="H122">
         <v>0</v>
@@ -7373,8 +7377,8 @@
       <c r="F123">
         <v>1</v>
       </c>
-      <c r="G123" t="s">
-        <v>19</v>
+      <c r="G123">
+        <v>1</v>
       </c>
       <c r="H123">
         <v>0</v>
@@ -7426,8 +7430,8 @@
       <c r="F124">
         <v>1</v>
       </c>
-      <c r="G124" t="s">
-        <v>19</v>
+      <c r="G124">
+        <v>1</v>
       </c>
       <c r="H124">
         <v>0</v>
@@ -7483,7 +7487,7 @@
         <v>1</v>
       </c>
       <c r="H125">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I125" t="s">
         <v>16</v>
@@ -7536,7 +7540,7 @@
         <v>1</v>
       </c>
       <c r="H126">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I126" t="s">
         <v>16</v>
@@ -7585,8 +7589,8 @@
       <c r="F127">
         <v>1</v>
       </c>
-      <c r="G127" t="s">
-        <v>19</v>
+      <c r="G127">
+        <v>1</v>
       </c>
       <c r="H127">
         <v>0</v>
@@ -7638,8 +7642,8 @@
       <c r="F128">
         <v>1</v>
       </c>
-      <c r="G128" t="s">
-        <v>19</v>
+      <c r="G128">
+        <v>1</v>
       </c>
       <c r="H128">
         <v>0</v>
@@ -7691,8 +7695,8 @@
       <c r="F129">
         <v>1</v>
       </c>
-      <c r="G129" t="s">
-        <v>19</v>
+      <c r="G129">
+        <v>1</v>
       </c>
       <c r="H129">
         <v>0</v>
@@ -7748,7 +7752,7 @@
         <v>5.1130685383596347E-5</v>
       </c>
       <c r="H130">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I130" t="s">
         <v>16</v>
@@ -8115,8 +8119,8 @@
       <c r="F137">
         <v>1</v>
       </c>
-      <c r="G137" t="s">
-        <v>19</v>
+      <c r="G137">
+        <v>1</v>
       </c>
       <c r="H137">
         <v>0</v>
@@ -8278,7 +8282,7 @@
         <v>1</v>
       </c>
       <c r="H140">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I140" t="s">
         <v>16</v>
@@ -8384,7 +8388,7 @@
         <v>1.1150758251561111E-3</v>
       </c>
       <c r="H142">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I142" t="s">
         <v>16</v>
@@ -8486,8 +8490,8 @@
       <c r="F144">
         <v>1</v>
       </c>
-      <c r="G144" t="s">
-        <v>19</v>
+      <c r="G144">
+        <v>1</v>
       </c>
       <c r="H144">
         <v>0</v>
@@ -8539,8 +8543,8 @@
       <c r="F145">
         <v>1</v>
       </c>
-      <c r="G145" t="s">
-        <v>19</v>
+      <c r="G145">
+        <v>1</v>
       </c>
       <c r="H145">
         <v>0</v>
@@ -8645,11 +8649,11 @@
       <c r="F147">
         <v>1</v>
       </c>
-      <c r="G147" t="s">
-        <v>19</v>
+      <c r="G147">
+        <v>1</v>
       </c>
       <c r="H147">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I147" t="s">
         <v>16</v>
@@ -8698,8 +8702,8 @@
       <c r="F148">
         <v>1</v>
       </c>
-      <c r="G148" t="s">
-        <v>19</v>
+      <c r="G148">
+        <v>1</v>
       </c>
       <c r="H148">
         <v>0</v>
@@ -9069,8 +9073,8 @@
       <c r="F155">
         <v>1</v>
       </c>
-      <c r="G155" t="s">
-        <v>19</v>
+      <c r="G155">
+        <v>1</v>
       </c>
       <c r="H155">
         <v>0</v>
@@ -9122,8 +9126,8 @@
       <c r="F156">
         <v>1</v>
       </c>
-      <c r="G156" t="s">
-        <v>19</v>
+      <c r="G156">
+        <v>1</v>
       </c>
       <c r="H156">
         <v>0</v>
@@ -9387,8 +9391,8 @@
       <c r="F161">
         <v>1</v>
       </c>
-      <c r="G161" t="s">
-        <v>19</v>
+      <c r="G161">
+        <v>1</v>
       </c>
       <c r="H161">
         <v>0</v>
@@ -9550,7 +9554,7 @@
         <v>1.685934489402697E-3</v>
       </c>
       <c r="H164">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I164" t="s">
         <v>16</v>
@@ -10076,8 +10080,8 @@
       <c r="F174">
         <v>1</v>
       </c>
-      <c r="G174" t="s">
-        <v>19</v>
+      <c r="G174">
+        <v>1</v>
       </c>
       <c r="H174">
         <v>0</v>
@@ -10129,8 +10133,8 @@
       <c r="F175">
         <v>1</v>
       </c>
-      <c r="G175" t="s">
-        <v>19</v>
+      <c r="G175">
+        <v>1</v>
       </c>
       <c r="H175">
         <v>0</v>
@@ -10538,8 +10542,8 @@
       <c r="F183">
         <v>1</v>
       </c>
-      <c r="G183" t="s">
-        <v>19</v>
+      <c r="G183">
+        <v>1</v>
       </c>
       <c r="H183">
         <v>0</v>
@@ -10591,8 +10595,8 @@
       <c r="F184">
         <v>1</v>
       </c>
-      <c r="G184" t="s">
-        <v>19</v>
+      <c r="G184">
+        <v>1</v>
       </c>
       <c r="H184">
         <v>0</v>
@@ -10644,8 +10648,8 @@
       <c r="F185">
         <v>1</v>
       </c>
-      <c r="G185" t="s">
-        <v>19</v>
+      <c r="G185">
+        <v>1</v>
       </c>
       <c r="H185">
         <v>0</v>
@@ -10697,8 +10701,8 @@
       <c r="F186">
         <v>1</v>
       </c>
-      <c r="G186" t="s">
-        <v>19</v>
+      <c r="G186">
+        <v>1</v>
       </c>
       <c r="H186">
         <v>0</v>
@@ -11174,8 +11178,8 @@
       <c r="F195">
         <v>1</v>
       </c>
-      <c r="G195" t="s">
-        <v>19</v>
+      <c r="G195">
+        <v>1</v>
       </c>
       <c r="H195">
         <v>0</v>
@@ -11227,8 +11231,8 @@
       <c r="F196">
         <v>1</v>
       </c>
-      <c r="G196" t="s">
-        <v>19</v>
+      <c r="G196">
+        <v>1</v>
       </c>
       <c r="H196">
         <v>0</v>
@@ -11280,8 +11284,8 @@
       <c r="F197">
         <v>1</v>
       </c>
-      <c r="G197" t="s">
-        <v>19</v>
+      <c r="G197">
+        <v>1</v>
       </c>
       <c r="H197">
         <v>0</v>
@@ -11492,8 +11496,8 @@
       <c r="F201">
         <v>1</v>
       </c>
-      <c r="G201" t="s">
-        <v>19</v>
+      <c r="G201">
+        <v>1</v>
       </c>
       <c r="H201">
         <v>0</v>
@@ -11651,8 +11655,8 @@
       <c r="F204">
         <v>1</v>
       </c>
-      <c r="G204" t="s">
-        <v>19</v>
+      <c r="G204">
+        <v>1</v>
       </c>
       <c r="H204">
         <v>0</v>
@@ -11810,8 +11814,8 @@
       <c r="F207">
         <v>1</v>
       </c>
-      <c r="G207" t="s">
-        <v>19</v>
+      <c r="G207">
+        <v>1</v>
       </c>
       <c r="H207">
         <v>0</v>
@@ -11916,8 +11920,8 @@
       <c r="F209">
         <v>1</v>
       </c>
-      <c r="G209" t="s">
-        <v>19</v>
+      <c r="G209">
+        <v>1</v>
       </c>
       <c r="H209">
         <v>0</v>
@@ -12022,8 +12026,8 @@
       <c r="F211">
         <v>1</v>
       </c>
-      <c r="G211" t="s">
-        <v>19</v>
+      <c r="G211">
+        <v>1</v>
       </c>
       <c r="H211">
         <v>0</v>
@@ -12234,8 +12238,8 @@
       <c r="F215">
         <v>1</v>
       </c>
-      <c r="G215" t="s">
-        <v>19</v>
+      <c r="G215">
+        <v>1</v>
       </c>
       <c r="H215">
         <v>0</v>
@@ -12446,8 +12450,8 @@
       <c r="F219">
         <v>1</v>
       </c>
-      <c r="G219" t="s">
-        <v>19</v>
+      <c r="G219">
+        <v>1</v>
       </c>
       <c r="H219">
         <v>0</v>
@@ -12499,8 +12503,8 @@
       <c r="F220">
         <v>1</v>
       </c>
-      <c r="G220" t="s">
-        <v>19</v>
+      <c r="G220">
+        <v>1</v>
       </c>
       <c r="H220">
         <v>0</v>
@@ -12605,8 +12609,8 @@
       <c r="F222">
         <v>1</v>
       </c>
-      <c r="G222" t="s">
-        <v>19</v>
+      <c r="G222">
+        <v>1</v>
       </c>
       <c r="H222">
         <v>0</v>
@@ -12658,8 +12662,8 @@
       <c r="F223">
         <v>1</v>
       </c>
-      <c r="G223" t="s">
-        <v>19</v>
+      <c r="G223">
+        <v>1</v>
       </c>
       <c r="H223">
         <v>0</v>
@@ -12711,8 +12715,8 @@
       <c r="F224">
         <v>1</v>
       </c>
-      <c r="G224" t="s">
-        <v>19</v>
+      <c r="G224">
+        <v>1</v>
       </c>
       <c r="H224">
         <v>0</v>
@@ -12764,8 +12768,8 @@
       <c r="F225">
         <v>1</v>
       </c>
-      <c r="G225" t="s">
-        <v>19</v>
+      <c r="G225">
+        <v>1</v>
       </c>
       <c r="H225">
         <v>0</v>
@@ -12817,8 +12821,8 @@
       <c r="F226">
         <v>1</v>
       </c>
-      <c r="G226" t="s">
-        <v>19</v>
+      <c r="G226">
+        <v>1</v>
       </c>
       <c r="H226">
         <v>0</v>
@@ -12923,8 +12927,8 @@
       <c r="F228">
         <v>1</v>
       </c>
-      <c r="G228" t="s">
-        <v>19</v>
+      <c r="G228">
+        <v>1</v>
       </c>
       <c r="H228">
         <v>0</v>
@@ -12976,8 +12980,8 @@
       <c r="F229">
         <v>1</v>
       </c>
-      <c r="G229" t="s">
-        <v>19</v>
+      <c r="G229">
+        <v>1</v>
       </c>
       <c r="H229">
         <v>0</v>
@@ -13029,8 +13033,8 @@
       <c r="F230">
         <v>1</v>
       </c>
-      <c r="G230" t="s">
-        <v>19</v>
+      <c r="G230">
+        <v>1</v>
       </c>
       <c r="H230">
         <v>0</v>
@@ -13082,8 +13086,8 @@
       <c r="F231">
         <v>1</v>
       </c>
-      <c r="G231" t="s">
-        <v>19</v>
+      <c r="G231">
+        <v>1</v>
       </c>
       <c r="H231">
         <v>0</v>
@@ -13135,8 +13139,8 @@
       <c r="F232">
         <v>1</v>
       </c>
-      <c r="G232" t="s">
-        <v>19</v>
+      <c r="G232">
+        <v>1</v>
       </c>
       <c r="H232">
         <v>0</v>
@@ -13188,8 +13192,8 @@
       <c r="F233">
         <v>1</v>
       </c>
-      <c r="G233" t="s">
-        <v>19</v>
+      <c r="G233">
+        <v>1</v>
       </c>
       <c r="H233">
         <v>0</v>
@@ -13241,8 +13245,8 @@
       <c r="F234">
         <v>1</v>
       </c>
-      <c r="G234" t="s">
-        <v>19</v>
+      <c r="G234">
+        <v>1</v>
       </c>
       <c r="H234">
         <v>0</v>
@@ -13294,8 +13298,8 @@
       <c r="F235">
         <v>1</v>
       </c>
-      <c r="G235" t="s">
-        <v>19</v>
+      <c r="G235">
+        <v>1</v>
       </c>
       <c r="H235">
         <v>0</v>
@@ -13347,8 +13351,8 @@
       <c r="F236">
         <v>1</v>
       </c>
-      <c r="G236" t="s">
-        <v>19</v>
+      <c r="G236">
+        <v>1</v>
       </c>
       <c r="H236">
         <v>0</v>
@@ -13400,8 +13404,8 @@
       <c r="F237">
         <v>1</v>
       </c>
-      <c r="G237" t="s">
-        <v>19</v>
+      <c r="G237">
+        <v>1</v>
       </c>
       <c r="H237">
         <v>0</v>
@@ -13453,8 +13457,8 @@
       <c r="F238">
         <v>1</v>
       </c>
-      <c r="G238" t="s">
-        <v>19</v>
+      <c r="G238">
+        <v>1</v>
       </c>
       <c r="H238">
         <v>0</v>
@@ -13506,8 +13510,8 @@
       <c r="F239">
         <v>1</v>
       </c>
-      <c r="G239" t="s">
-        <v>19</v>
+      <c r="G239">
+        <v>1</v>
       </c>
       <c r="H239">
         <v>0</v>
@@ -13559,8 +13563,8 @@
       <c r="F240">
         <v>1</v>
       </c>
-      <c r="G240" t="s">
-        <v>19</v>
+      <c r="G240">
+        <v>1</v>
       </c>
       <c r="H240">
         <v>0</v>
@@ -13612,8 +13616,8 @@
       <c r="F241">
         <v>1</v>
       </c>
-      <c r="G241" t="s">
-        <v>19</v>
+      <c r="G241">
+        <v>1</v>
       </c>
       <c r="H241">
         <v>0</v>
@@ -13665,8 +13669,8 @@
       <c r="F242">
         <v>1</v>
       </c>
-      <c r="G242" t="s">
-        <v>19</v>
+      <c r="G242">
+        <v>1</v>
       </c>
       <c r="H242">
         <v>0</v>
@@ -13718,8 +13722,8 @@
       <c r="F243">
         <v>1</v>
       </c>
-      <c r="G243" t="s">
-        <v>19</v>
+      <c r="G243">
+        <v>1</v>
       </c>
       <c r="H243">
         <v>0</v>
@@ -13771,8 +13775,8 @@
       <c r="F244">
         <v>1</v>
       </c>
-      <c r="G244" t="s">
-        <v>19</v>
+      <c r="G244">
+        <v>1</v>
       </c>
       <c r="H244">
         <v>0</v>
@@ -13824,8 +13828,8 @@
       <c r="F245">
         <v>1</v>
       </c>
-      <c r="G245" t="s">
-        <v>19</v>
+      <c r="G245">
+        <v>1</v>
       </c>
       <c r="H245">
         <v>0</v>
@@ -13877,8 +13881,8 @@
       <c r="F246">
         <v>1</v>
       </c>
-      <c r="G246" t="s">
-        <v>19</v>
+      <c r="G246">
+        <v>1</v>
       </c>
       <c r="H246">
         <v>0</v>
@@ -13983,8 +13987,8 @@
       <c r="F248">
         <v>1</v>
       </c>
-      <c r="G248" t="s">
-        <v>19</v>
+      <c r="G248">
+        <v>1</v>
       </c>
       <c r="H248">
         <v>0</v>
@@ -14089,8 +14093,8 @@
       <c r="F250">
         <v>1</v>
       </c>
-      <c r="G250" t="s">
-        <v>19</v>
+      <c r="G250">
+        <v>1</v>
       </c>
       <c r="H250">
         <v>0</v>
@@ -14248,8 +14252,8 @@
       <c r="F253">
         <v>1</v>
       </c>
-      <c r="G253" t="s">
-        <v>19</v>
+      <c r="G253">
+        <v>1</v>
       </c>
       <c r="H253">
         <v>0</v>
@@ -14301,8 +14305,8 @@
       <c r="F254">
         <v>1</v>
       </c>
-      <c r="G254" t="s">
-        <v>19</v>
+      <c r="G254">
+        <v>1</v>
       </c>
       <c r="H254">
         <v>0</v>
@@ -14354,8 +14358,8 @@
       <c r="F255">
         <v>1</v>
       </c>
-      <c r="G255" t="s">
-        <v>19</v>
+      <c r="G255">
+        <v>1</v>
       </c>
       <c r="H255">
         <v>0</v>
@@ -14407,8 +14411,8 @@
       <c r="F256">
         <v>1</v>
       </c>
-      <c r="G256" t="s">
-        <v>19</v>
+      <c r="G256">
+        <v>1</v>
       </c>
       <c r="H256">
         <v>0</v>
@@ -14460,8 +14464,8 @@
       <c r="F257">
         <v>1</v>
       </c>
-      <c r="G257" t="s">
-        <v>19</v>
+      <c r="G257">
+        <v>1</v>
       </c>
       <c r="H257">
         <v>0</v>
@@ -14513,8 +14517,8 @@
       <c r="F258">
         <v>1</v>
       </c>
-      <c r="G258" t="s">
-        <v>19</v>
+      <c r="G258">
+        <v>1</v>
       </c>
       <c r="H258">
         <v>0</v>
@@ -14566,8 +14570,8 @@
       <c r="F259">
         <v>1</v>
       </c>
-      <c r="G259" t="s">
-        <v>19</v>
+      <c r="G259">
+        <v>1</v>
       </c>
       <c r="H259">
         <v>0</v>
@@ -14619,8 +14623,8 @@
       <c r="F260">
         <v>1</v>
       </c>
-      <c r="G260" t="s">
-        <v>19</v>
+      <c r="G260">
+        <v>1</v>
       </c>
       <c r="H260">
         <v>0</v>
@@ -14672,8 +14676,8 @@
       <c r="F261">
         <v>1</v>
       </c>
-      <c r="G261" t="s">
-        <v>19</v>
+      <c r="G261">
+        <v>1</v>
       </c>
       <c r="H261">
         <v>0</v>
@@ -14725,8 +14729,8 @@
       <c r="F262">
         <v>1</v>
       </c>
-      <c r="G262" t="s">
-        <v>19</v>
+      <c r="G262">
+        <v>1</v>
       </c>
       <c r="H262">
         <v>0</v>
@@ -14937,8 +14941,8 @@
       <c r="F266">
         <v>1</v>
       </c>
-      <c r="G266" t="s">
-        <v>19</v>
+      <c r="G266">
+        <v>1</v>
       </c>
       <c r="H266">
         <v>0</v>
@@ -15202,8 +15206,8 @@
       <c r="F271">
         <v>1</v>
       </c>
-      <c r="G271" t="s">
-        <v>19</v>
+      <c r="G271">
+        <v>1</v>
       </c>
       <c r="H271">
         <v>0</v>
@@ -15255,8 +15259,8 @@
       <c r="F272">
         <v>1</v>
       </c>
-      <c r="G272" t="s">
-        <v>19</v>
+      <c r="G272">
+        <v>1</v>
       </c>
       <c r="H272">
         <v>0</v>
@@ -15471,7 +15475,7 @@
         <v>1.5043249341857841E-3</v>
       </c>
       <c r="H276">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I276" t="s">
         <v>16</v>
@@ -15679,8 +15683,8 @@
       <c r="F280">
         <v>1</v>
       </c>
-      <c r="G280" t="s">
-        <v>19</v>
+      <c r="G280">
+        <v>1</v>
       </c>
       <c r="H280">
         <v>0</v>
@@ -15732,8 +15736,8 @@
       <c r="F281">
         <v>1</v>
       </c>
-      <c r="G281" t="s">
-        <v>19</v>
+      <c r="G281">
+        <v>1</v>
       </c>
       <c r="H281">
         <v>1</v>
@@ -15838,8 +15842,8 @@
       <c r="F283">
         <v>1</v>
       </c>
-      <c r="G283" t="s">
-        <v>19</v>
+      <c r="G283">
+        <v>1</v>
       </c>
       <c r="H283">
         <v>0</v>
@@ -15944,8 +15948,8 @@
       <c r="F285">
         <v>1</v>
       </c>
-      <c r="G285" t="s">
-        <v>19</v>
+      <c r="G285">
+        <v>1</v>
       </c>
       <c r="H285">
         <v>0</v>
@@ -16047,8 +16051,8 @@
       <c r="F287">
         <v>1</v>
       </c>
-      <c r="G287" t="s">
-        <v>19</v>
+      <c r="G287">
+        <v>1</v>
       </c>
       <c r="H287">
         <v>0</v>
@@ -16210,7 +16214,7 @@
         <v>8.4459459459459464E-4</v>
       </c>
       <c r="H290">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I290" t="s">
         <v>16</v>
@@ -16880,8 +16884,8 @@
       <c r="F303">
         <v>1</v>
       </c>
-      <c r="G303" t="s">
-        <v>19</v>
+      <c r="G303">
+        <v>1</v>
       </c>
       <c r="H303">
         <v>0</v>
@@ -16933,8 +16937,8 @@
       <c r="F304">
         <v>1</v>
       </c>
-      <c r="G304" t="s">
-        <v>19</v>
+      <c r="G304">
+        <v>1</v>
       </c>
       <c r="H304">
         <v>0</v>
@@ -17092,8 +17096,8 @@
       <c r="F307">
         <v>1</v>
       </c>
-      <c r="G307" t="s">
-        <v>19</v>
+      <c r="G307">
+        <v>1</v>
       </c>
       <c r="H307">
         <v>0</v>
@@ -17145,8 +17149,8 @@
       <c r="F308">
         <v>1</v>
       </c>
-      <c r="G308" t="s">
-        <v>19</v>
+      <c r="G308">
+        <v>1</v>
       </c>
       <c r="H308">
         <v>0</v>
@@ -17198,8 +17202,8 @@
       <c r="F309">
         <v>1</v>
       </c>
-      <c r="G309" t="s">
-        <v>19</v>
+      <c r="G309">
+        <v>1</v>
       </c>
       <c r="H309">
         <v>0</v>
@@ -17675,8 +17679,8 @@
       <c r="F318">
         <v>1</v>
       </c>
-      <c r="G318" t="s">
-        <v>19</v>
+      <c r="G318">
+        <v>1</v>
       </c>
       <c r="H318">
         <v>0</v>
@@ -17728,8 +17732,8 @@
       <c r="F319">
         <v>1</v>
       </c>
-      <c r="G319" t="s">
-        <v>19</v>
+      <c r="G319">
+        <v>1</v>
       </c>
       <c r="H319">
         <v>0</v>
@@ -17781,8 +17785,8 @@
       <c r="F320">
         <v>1</v>
       </c>
-      <c r="G320" t="s">
-        <v>19</v>
+      <c r="G320">
+        <v>1</v>
       </c>
       <c r="H320">
         <v>0</v>
@@ -17834,8 +17838,8 @@
       <c r="F321">
         <v>1</v>
       </c>
-      <c r="G321" t="s">
-        <v>19</v>
+      <c r="G321">
+        <v>1</v>
       </c>
       <c r="H321">
         <v>0</v>
@@ -17887,8 +17891,8 @@
       <c r="F322">
         <v>1</v>
       </c>
-      <c r="G322" t="s">
-        <v>19</v>
+      <c r="G322">
+        <v>1</v>
       </c>
       <c r="H322">
         <v>0</v>
@@ -18523,8 +18527,8 @@
       <c r="F334">
         <v>1</v>
       </c>
-      <c r="G334" t="s">
-        <v>19</v>
+      <c r="G334">
+        <v>1</v>
       </c>
       <c r="H334">
         <v>0</v>
@@ -18682,8 +18686,8 @@
       <c r="F337">
         <v>1</v>
       </c>
-      <c r="G337" t="s">
-        <v>19</v>
+      <c r="G337">
+        <v>1</v>
       </c>
       <c r="H337">
         <v>0</v>
@@ -18735,8 +18739,8 @@
       <c r="F338">
         <v>1</v>
       </c>
-      <c r="G338" t="s">
-        <v>19</v>
+      <c r="G338">
+        <v>1</v>
       </c>
       <c r="H338">
         <v>0</v>
@@ -19153,8 +19157,8 @@
       <c r="F346">
         <v>1</v>
       </c>
-      <c r="G346" t="s">
-        <v>19</v>
+      <c r="G346">
+        <v>1</v>
       </c>
       <c r="H346">
         <v>0</v>
@@ -19206,8 +19210,8 @@
       <c r="F347">
         <v>1</v>
       </c>
-      <c r="G347" t="s">
-        <v>19</v>
+      <c r="G347">
+        <v>1</v>
       </c>
       <c r="H347">
         <v>0</v>
@@ -19259,8 +19263,8 @@
       <c r="F348">
         <v>1</v>
       </c>
-      <c r="G348" t="s">
-        <v>19</v>
+      <c r="G348">
+        <v>1</v>
       </c>
       <c r="H348">
         <v>0</v>
@@ -19312,8 +19316,8 @@
       <c r="F349">
         <v>1</v>
       </c>
-      <c r="G349" t="s">
-        <v>19</v>
+      <c r="G349">
+        <v>1</v>
       </c>
       <c r="H349">
         <v>0</v>
@@ -19365,8 +19369,8 @@
       <c r="F350">
         <v>1</v>
       </c>
-      <c r="G350" t="s">
-        <v>19</v>
+      <c r="G350">
+        <v>1</v>
       </c>
       <c r="H350">
         <v>0</v>
@@ -19422,7 +19426,7 @@
         <v>1.7116626468528749E-4</v>
       </c>
       <c r="H351">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I351" t="s">
         <v>16</v>
@@ -19789,8 +19793,8 @@
       <c r="F358">
         <v>1</v>
       </c>
-      <c r="G358" t="s">
-        <v>19</v>
+      <c r="G358">
+        <v>1</v>
       </c>
       <c r="H358">
         <v>0</v>
@@ -20160,8 +20164,8 @@
       <c r="F365">
         <v>1</v>
       </c>
-      <c r="G365" t="s">
-        <v>19</v>
+      <c r="G365">
+        <v>1</v>
       </c>
       <c r="H365">
         <v>0</v>
@@ -20266,8 +20270,8 @@
       <c r="F367">
         <v>1</v>
       </c>
-      <c r="G367" t="s">
-        <v>19</v>
+      <c r="G367">
+        <v>1</v>
       </c>
       <c r="H367">
         <v>0</v>
@@ -20319,8 +20323,8 @@
       <c r="F368">
         <v>1</v>
       </c>
-      <c r="G368" t="s">
-        <v>19</v>
+      <c r="G368">
+        <v>1</v>
       </c>
       <c r="H368">
         <v>0</v>
@@ -20372,8 +20376,8 @@
       <c r="F369">
         <v>1</v>
       </c>
-      <c r="G369" t="s">
-        <v>19</v>
+      <c r="G369">
+        <v>1</v>
       </c>
       <c r="H369">
         <v>0</v>
@@ -20425,8 +20429,8 @@
       <c r="F370">
         <v>1</v>
       </c>
-      <c r="G370" t="s">
-        <v>19</v>
+      <c r="G370">
+        <v>1</v>
       </c>
       <c r="H370">
         <v>0</v>
@@ -20478,8 +20482,8 @@
       <c r="F371">
         <v>1</v>
       </c>
-      <c r="G371" t="s">
-        <v>19</v>
+      <c r="G371">
+        <v>1</v>
       </c>
       <c r="H371">
         <v>0</v>
@@ -20531,8 +20535,8 @@
       <c r="F372">
         <v>1</v>
       </c>
-      <c r="G372" t="s">
-        <v>19</v>
+      <c r="G372">
+        <v>1</v>
       </c>
       <c r="H372">
         <v>0</v>
@@ -20584,8 +20588,8 @@
       <c r="F373">
         <v>1</v>
       </c>
-      <c r="G373" t="s">
-        <v>19</v>
+      <c r="G373">
+        <v>1</v>
       </c>
       <c r="H373">
         <v>0</v>
@@ -20690,8 +20694,8 @@
       <c r="F375">
         <v>1</v>
       </c>
-      <c r="G375" t="s">
-        <v>19</v>
+      <c r="G375">
+        <v>1</v>
       </c>
       <c r="H375">
         <v>0</v>
@@ -20849,8 +20853,8 @@
       <c r="F378">
         <v>1</v>
       </c>
-      <c r="G378" t="s">
-        <v>19</v>
+      <c r="G378">
+        <v>1</v>
       </c>
       <c r="H378">
         <v>0</v>
@@ -21008,8 +21012,8 @@
       <c r="F381">
         <v>1</v>
       </c>
-      <c r="G381" t="s">
-        <v>19</v>
+      <c r="G381">
+        <v>1</v>
       </c>
       <c r="H381">
         <v>0</v>
@@ -21330,7 +21334,7 @@
         <v>1.013787510137875E-4</v>
       </c>
       <c r="H387">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I387" t="s">
         <v>16</v>
@@ -21803,8 +21807,8 @@
       <c r="F396">
         <v>1</v>
       </c>
-      <c r="G396" t="s">
-        <v>19</v>
+      <c r="G396">
+        <v>1</v>
       </c>
       <c r="H396">
         <v>0</v>
@@ -21856,8 +21860,8 @@
       <c r="F397">
         <v>1</v>
       </c>
-      <c r="G397" t="s">
-        <v>19</v>
+      <c r="G397">
+        <v>1</v>
       </c>
       <c r="H397">
         <v>0</v>
@@ -21909,8 +21913,8 @@
       <c r="F398">
         <v>1</v>
       </c>
-      <c r="G398" t="s">
-        <v>19</v>
+      <c r="G398">
+        <v>1</v>
       </c>
       <c r="H398">
         <v>0</v>
@@ -21962,8 +21966,8 @@
       <c r="F399">
         <v>1</v>
       </c>
-      <c r="G399" t="s">
-        <v>19</v>
+      <c r="G399">
+        <v>1</v>
       </c>
       <c r="H399">
         <v>0</v>
@@ -22015,8 +22019,8 @@
       <c r="F400">
         <v>1</v>
       </c>
-      <c r="G400" t="s">
-        <v>19</v>
+      <c r="G400">
+        <v>1</v>
       </c>
       <c r="H400">
         <v>0</v>
@@ -22068,8 +22072,8 @@
       <c r="F401">
         <v>1</v>
       </c>
-      <c r="G401" t="s">
-        <v>19</v>
+      <c r="G401">
+        <v>1</v>
       </c>
       <c r="H401">
         <v>0</v>
@@ -22174,8 +22178,8 @@
       <c r="F403">
         <v>1</v>
       </c>
-      <c r="G403" t="s">
-        <v>19</v>
+      <c r="G403">
+        <v>1</v>
       </c>
       <c r="H403">
         <v>0</v>
@@ -22383,8 +22387,8 @@
       <c r="F407">
         <v>1</v>
       </c>
-      <c r="G407" t="s">
-        <v>19</v>
+      <c r="G407">
+        <v>1</v>
       </c>
       <c r="H407">
         <v>0</v>
@@ -22436,8 +22440,8 @@
       <c r="F408">
         <v>1</v>
       </c>
-      <c r="G408" t="s">
-        <v>19</v>
+      <c r="G408">
+        <v>1</v>
       </c>
       <c r="H408">
         <v>0</v>
@@ -22489,8 +22493,8 @@
       <c r="F409">
         <v>1</v>
       </c>
-      <c r="G409" t="s">
-        <v>19</v>
+      <c r="G409">
+        <v>1</v>
       </c>
       <c r="H409">
         <v>0</v>
@@ -22542,8 +22546,8 @@
       <c r="F410">
         <v>1</v>
       </c>
-      <c r="G410" t="s">
-        <v>19</v>
+      <c r="G410">
+        <v>1</v>
       </c>
       <c r="H410">
         <v>0</v>
@@ -22648,8 +22652,8 @@
       <c r="F412">
         <v>1</v>
       </c>
-      <c r="G412" t="s">
-        <v>19</v>
+      <c r="G412">
+        <v>1</v>
       </c>
       <c r="H412">
         <v>0</v>
@@ -22701,8 +22705,8 @@
       <c r="F413">
         <v>1</v>
       </c>
-      <c r="G413" t="s">
-        <v>19</v>
+      <c r="G413">
+        <v>1</v>
       </c>
       <c r="H413">
         <v>0</v>
@@ -22754,8 +22758,8 @@
       <c r="F414">
         <v>1</v>
       </c>
-      <c r="G414" t="s">
-        <v>19</v>
+      <c r="G414">
+        <v>1</v>
       </c>
       <c r="H414">
         <v>0</v>
@@ -22807,8 +22811,8 @@
       <c r="F415">
         <v>1</v>
       </c>
-      <c r="G415" t="s">
-        <v>19</v>
+      <c r="G415">
+        <v>1</v>
       </c>
       <c r="H415">
         <v>0</v>
@@ -22860,8 +22864,8 @@
       <c r="F416">
         <v>1</v>
       </c>
-      <c r="G416" t="s">
-        <v>19</v>
+      <c r="G416">
+        <v>1</v>
       </c>
       <c r="H416">
         <v>0</v>
@@ -22966,8 +22970,8 @@
       <c r="F418">
         <v>1</v>
       </c>
-      <c r="G418" t="s">
-        <v>19</v>
+      <c r="G418">
+        <v>1</v>
       </c>
       <c r="H418">
         <v>0</v>
@@ -23019,8 +23023,8 @@
       <c r="F419">
         <v>1</v>
       </c>
-      <c r="G419" t="s">
-        <v>19</v>
+      <c r="G419">
+        <v>1</v>
       </c>
       <c r="H419">
         <v>0</v>
@@ -23125,8 +23129,8 @@
       <c r="F421">
         <v>1</v>
       </c>
-      <c r="G421" t="s">
-        <v>19</v>
+      <c r="G421">
+        <v>1</v>
       </c>
       <c r="H421">
         <v>0</v>
@@ -23178,8 +23182,8 @@
       <c r="F422">
         <v>1</v>
       </c>
-      <c r="G422" t="s">
-        <v>19</v>
+      <c r="G422">
+        <v>1</v>
       </c>
       <c r="H422">
         <v>0</v>
@@ -23231,8 +23235,8 @@
       <c r="F423">
         <v>1</v>
       </c>
-      <c r="G423" t="s">
-        <v>19</v>
+      <c r="G423">
+        <v>1</v>
       </c>
       <c r="H423">
         <v>0</v>
@@ -23284,8 +23288,8 @@
       <c r="F424">
         <v>1</v>
       </c>
-      <c r="G424" t="s">
-        <v>19</v>
+      <c r="G424">
+        <v>1</v>
       </c>
       <c r="H424">
         <v>0</v>
@@ -23337,8 +23341,8 @@
       <c r="F425">
         <v>1</v>
       </c>
-      <c r="G425" t="s">
-        <v>19</v>
+      <c r="G425">
+        <v>1</v>
       </c>
       <c r="H425">
         <v>0</v>
@@ -23390,8 +23394,8 @@
       <c r="F426">
         <v>1</v>
       </c>
-      <c r="G426" t="s">
-        <v>19</v>
+      <c r="G426">
+        <v>1</v>
       </c>
       <c r="H426">
         <v>0</v>
@@ -23602,8 +23606,8 @@
       <c r="F430">
         <v>1</v>
       </c>
-      <c r="G430" t="s">
-        <v>19</v>
+      <c r="G430">
+        <v>1</v>
       </c>
       <c r="H430">
         <v>0</v>
@@ -23761,8 +23765,8 @@
       <c r="F433">
         <v>1</v>
       </c>
-      <c r="G433" t="s">
-        <v>19</v>
+      <c r="G433">
+        <v>1</v>
       </c>
       <c r="H433">
         <v>0</v>
@@ -23814,8 +23818,8 @@
       <c r="F434">
         <v>1</v>
       </c>
-      <c r="G434" t="s">
-        <v>19</v>
+      <c r="G434">
+        <v>1</v>
       </c>
       <c r="H434">
         <v>0</v>
@@ -23973,8 +23977,8 @@
       <c r="F437">
         <v>1</v>
       </c>
-      <c r="G437" t="s">
-        <v>19</v>
+      <c r="G437">
+        <v>1</v>
       </c>
       <c r="H437">
         <v>0</v>
@@ -24026,8 +24030,8 @@
       <c r="F438">
         <v>1</v>
       </c>
-      <c r="G438" t="s">
-        <v>19</v>
+      <c r="G438">
+        <v>1</v>
       </c>
       <c r="H438">
         <v>0</v>
@@ -24083,7 +24087,7 @@
         <v>7.5502779875077214E-4</v>
       </c>
       <c r="H439">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I439" t="s">
         <v>16</v>
@@ -24450,8 +24454,8 @@
       <c r="F446">
         <v>1</v>
       </c>
-      <c r="G446" t="s">
-        <v>19</v>
+      <c r="G446">
+        <v>1</v>
       </c>
       <c r="H446">
         <v>0</v>
@@ -24613,7 +24617,7 @@
         <v>4.3092303714556583E-5</v>
       </c>
       <c r="H449">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I449" t="s">
         <v>22</v>
@@ -24662,8 +24666,8 @@
       <c r="F450">
         <v>1</v>
       </c>
-      <c r="G450" t="s">
-        <v>19</v>
+      <c r="G450">
+        <v>1</v>
       </c>
       <c r="H450">
         <v>0</v>
@@ -24821,8 +24825,8 @@
       <c r="F453">
         <v>1</v>
       </c>
-      <c r="G453" t="s">
-        <v>19</v>
+      <c r="G453">
+        <v>1</v>
       </c>
       <c r="H453">
         <v>0</v>
@@ -24980,8 +24984,8 @@
       <c r="F456">
         <v>1</v>
       </c>
-      <c r="G456" t="s">
-        <v>19</v>
+      <c r="G456">
+        <v>1</v>
       </c>
       <c r="H456">
         <v>0</v>
@@ -25086,8 +25090,8 @@
       <c r="F458">
         <v>1</v>
       </c>
-      <c r="G458" t="s">
-        <v>19</v>
+      <c r="G458">
+        <v>1</v>
       </c>
       <c r="H458">
         <v>0</v>
@@ -25139,8 +25143,8 @@
       <c r="F459">
         <v>1</v>
       </c>
-      <c r="G459" t="s">
-        <v>19</v>
+      <c r="G459">
+        <v>1</v>
       </c>
       <c r="H459">
         <v>0</v>
@@ -25192,8 +25196,8 @@
       <c r="F460">
         <v>1</v>
       </c>
-      <c r="G460" t="s">
-        <v>19</v>
+      <c r="G460">
+        <v>1</v>
       </c>
       <c r="H460">
         <v>0</v>
@@ -25245,8 +25249,8 @@
       <c r="F461">
         <v>1</v>
       </c>
-      <c r="G461" t="s">
-        <v>19</v>
+      <c r="G461">
+        <v>1</v>
       </c>
       <c r="H461">
         <v>0</v>
@@ -25461,7 +25465,7 @@
         <v>4.0001600064002562E-5</v>
       </c>
       <c r="H465">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I465" t="s">
         <v>22</v>
@@ -25510,8 +25514,8 @@
       <c r="F466">
         <v>1</v>
       </c>
-      <c r="G466" t="s">
-        <v>19</v>
+      <c r="G466">
+        <v>1</v>
       </c>
       <c r="H466">
         <v>0</v>
@@ -25669,8 +25673,8 @@
       <c r="F469">
         <v>1</v>
       </c>
-      <c r="G469" t="s">
-        <v>19</v>
+      <c r="G469">
+        <v>1</v>
       </c>
       <c r="H469">
         <v>0</v>
@@ -25828,8 +25832,8 @@
       <c r="F472">
         <v>1</v>
       </c>
-      <c r="G472" t="s">
-        <v>19</v>
+      <c r="G472">
+        <v>1</v>
       </c>
       <c r="H472">
         <v>0</v>
@@ -25934,8 +25938,8 @@
       <c r="F474">
         <v>1</v>
       </c>
-      <c r="G474" t="s">
-        <v>19</v>
+      <c r="G474">
+        <v>1</v>
       </c>
       <c r="H474">
         <v>0</v>
@@ -25987,8 +25991,8 @@
       <c r="F475">
         <v>1</v>
       </c>
-      <c r="G475" t="s">
-        <v>19</v>
+      <c r="G475">
+        <v>1</v>
       </c>
       <c r="H475">
         <v>0</v>
@@ -26040,8 +26044,8 @@
       <c r="F476">
         <v>1</v>
       </c>
-      <c r="G476" t="s">
-        <v>19</v>
+      <c r="G476">
+        <v>1</v>
       </c>
       <c r="H476">
         <v>0</v>
@@ -26093,8 +26097,8 @@
       <c r="F477">
         <v>1</v>
       </c>
-      <c r="G477" t="s">
-        <v>19</v>
+      <c r="G477">
+        <v>1</v>
       </c>
       <c r="H477">
         <v>0</v>
@@ -26199,8 +26203,8 @@
       <c r="F479">
         <v>1</v>
       </c>
-      <c r="G479" t="s">
-        <v>19</v>
+      <c r="G479">
+        <v>1</v>
       </c>
       <c r="H479">
         <v>0</v>
@@ -26305,8 +26309,8 @@
       <c r="F481">
         <v>1</v>
       </c>
-      <c r="G481" t="s">
-        <v>19</v>
+      <c r="G481">
+        <v>1</v>
       </c>
       <c r="H481">
         <v>0</v>
@@ -26517,8 +26521,8 @@
       <c r="F485">
         <v>1</v>
       </c>
-      <c r="G485" t="s">
-        <v>19</v>
+      <c r="G485">
+        <v>1</v>
       </c>
       <c r="H485">
         <v>0</v>
@@ -26729,8 +26733,8 @@
       <c r="F489">
         <v>1</v>
       </c>
-      <c r="G489" t="s">
-        <v>19</v>
+      <c r="G489">
+        <v>1</v>
       </c>
       <c r="H489">
         <v>0</v>
@@ -26782,8 +26786,8 @@
       <c r="F490">
         <v>1</v>
       </c>
-      <c r="G490" t="s">
-        <v>19</v>
+      <c r="G490">
+        <v>1</v>
       </c>
       <c r="H490">
         <v>0</v>
@@ -26892,7 +26896,7 @@
         <v>3.8270919841558389E-5</v>
       </c>
       <c r="H492">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I492" t="s">
         <v>22</v>
@@ -26941,8 +26945,8 @@
       <c r="F493">
         <v>1</v>
       </c>
-      <c r="G493" t="s">
-        <v>19</v>
+      <c r="G493">
+        <v>1</v>
       </c>
       <c r="H493">
         <v>0</v>
@@ -27100,8 +27104,8 @@
       <c r="F496">
         <v>1</v>
       </c>
-      <c r="G496" t="s">
-        <v>19</v>
+      <c r="G496">
+        <v>1</v>
       </c>
       <c r="H496">
         <v>0</v>
@@ -27259,8 +27263,8 @@
       <c r="F499">
         <v>1</v>
       </c>
-      <c r="G499" t="s">
-        <v>19</v>
+      <c r="G499">
+        <v>1</v>
       </c>
       <c r="H499">
         <v>0</v>
@@ -27365,8 +27369,8 @@
       <c r="F501">
         <v>1</v>
       </c>
-      <c r="G501" t="s">
-        <v>19</v>
+      <c r="G501">
+        <v>1</v>
       </c>
       <c r="H501">
         <v>0</v>
@@ -27418,8 +27422,8 @@
       <c r="F502">
         <v>1</v>
       </c>
-      <c r="G502" t="s">
-        <v>19</v>
+      <c r="G502">
+        <v>1</v>
       </c>
       <c r="H502">
         <v>0</v>
@@ -27471,8 +27475,8 @@
       <c r="F503">
         <v>1</v>
       </c>
-      <c r="G503" t="s">
-        <v>19</v>
+      <c r="G503">
+        <v>1</v>
       </c>
       <c r="H503">
         <v>0</v>
@@ -27524,8 +27528,8 @@
       <c r="F504">
         <v>1</v>
       </c>
-      <c r="G504" t="s">
-        <v>19</v>
+      <c r="G504">
+        <v>1</v>
       </c>
       <c r="H504">
         <v>0</v>
@@ -27793,7 +27797,7 @@
         <v>5.1413881748071976E-4</v>
       </c>
       <c r="H509">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I509" t="s">
         <v>16</v>
@@ -27895,8 +27899,8 @@
       <c r="F511">
         <v>1</v>
       </c>
-      <c r="G511" t="s">
-        <v>19</v>
+      <c r="G511">
+        <v>1</v>
       </c>
       <c r="H511">
         <v>0</v>
@@ -27948,8 +27952,8 @@
       <c r="F512">
         <v>1</v>
       </c>
-      <c r="G512" t="s">
-        <v>19</v>
+      <c r="G512">
+        <v>1</v>
       </c>
       <c r="H512">
         <v>0</v>
@@ -28058,7 +28062,7 @@
         <v>9.4339622641509441E-2</v>
       </c>
       <c r="H514">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I514" t="s">
         <v>16</v>
@@ -28323,7 +28327,7 @@
         <v>1.336541031809677E-3</v>
       </c>
       <c r="H519">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I519" t="s">
         <v>16</v>
@@ -28372,8 +28376,8 @@
       <c r="F520">
         <v>1</v>
       </c>
-      <c r="G520" t="s">
-        <v>19</v>
+      <c r="G520">
+        <v>1</v>
       </c>
       <c r="H520">
         <v>0</v>
@@ -28425,8 +28429,8 @@
       <c r="F521">
         <v>1</v>
       </c>
-      <c r="G521" t="s">
-        <v>19</v>
+      <c r="G521">
+        <v>1</v>
       </c>
       <c r="H521">
         <v>0</v>
@@ -28478,8 +28482,8 @@
       <c r="F522">
         <v>1</v>
       </c>
-      <c r="G522" t="s">
-        <v>19</v>
+      <c r="G522">
+        <v>1</v>
       </c>
       <c r="H522">
         <v>0</v>
@@ -28637,8 +28641,8 @@
       <c r="F525">
         <v>1</v>
       </c>
-      <c r="G525" t="s">
-        <v>19</v>
+      <c r="G525">
+        <v>1</v>
       </c>
       <c r="H525">
         <v>0</v>
@@ -28743,8 +28747,8 @@
       <c r="F527">
         <v>1</v>
       </c>
-      <c r="G527" t="s">
-        <v>19</v>
+      <c r="G527">
+        <v>1</v>
       </c>
       <c r="H527">
         <v>0</v>
@@ -28853,7 +28857,7 @@
         <v>4.0364898684104301E-5</v>
       </c>
       <c r="H529">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I529" t="s">
         <v>22</v>
@@ -28902,8 +28906,8 @@
       <c r="F530">
         <v>1</v>
       </c>
-      <c r="G530" t="s">
-        <v>19</v>
+      <c r="G530">
+        <v>1</v>
       </c>
       <c r="H530">
         <v>0</v>
@@ -29061,8 +29065,8 @@
       <c r="F533">
         <v>1</v>
       </c>
-      <c r="G533" t="s">
-        <v>19</v>
+      <c r="G533">
+        <v>1</v>
       </c>
       <c r="H533">
         <v>0</v>
@@ -29220,8 +29224,8 @@
       <c r="F536">
         <v>1</v>
       </c>
-      <c r="G536" t="s">
-        <v>19</v>
+      <c r="G536">
+        <v>1</v>
       </c>
       <c r="H536">
         <v>0</v>
@@ -29326,8 +29330,8 @@
       <c r="F538">
         <v>1</v>
       </c>
-      <c r="G538" t="s">
-        <v>19</v>
+      <c r="G538">
+        <v>1</v>
       </c>
       <c r="H538">
         <v>0</v>
@@ -29379,8 +29383,8 @@
       <c r="F539">
         <v>1</v>
       </c>
-      <c r="G539" t="s">
-        <v>19</v>
+      <c r="G539">
+        <v>1</v>
       </c>
       <c r="H539">
         <v>0</v>
@@ -29432,8 +29436,8 @@
       <c r="F540">
         <v>1</v>
       </c>
-      <c r="G540" t="s">
-        <v>19</v>
+      <c r="G540">
+        <v>1</v>
       </c>
       <c r="H540">
         <v>0</v>
@@ -29489,7 +29493,7 @@
         <v>9.4339622641509441E-2</v>
       </c>
       <c r="H541">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I541" t="s">
         <v>16</v>
@@ -29754,7 +29758,7 @@
         <v>1.1173184357541901E-3</v>
       </c>
       <c r="H546">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I546" t="s">
         <v>16</v>
@@ -29803,8 +29807,8 @@
       <c r="F547">
         <v>1</v>
       </c>
-      <c r="G547" t="s">
-        <v>19</v>
+      <c r="G547">
+        <v>1</v>
       </c>
       <c r="H547">
         <v>0</v>
@@ -29856,8 +29860,8 @@
       <c r="F548">
         <v>1</v>
       </c>
-      <c r="G548" t="s">
-        <v>19</v>
+      <c r="G548">
+        <v>1</v>
       </c>
       <c r="H548">
         <v>0</v>
@@ -29909,8 +29913,8 @@
       <c r="F549">
         <v>1</v>
       </c>
-      <c r="G549" t="s">
-        <v>19</v>
+      <c r="G549">
+        <v>1</v>
       </c>
       <c r="H549">
         <v>0</v>
@@ -30068,8 +30072,8 @@
       <c r="F552">
         <v>1</v>
       </c>
-      <c r="G552" t="s">
-        <v>19</v>
+      <c r="G552">
+        <v>1</v>
       </c>
       <c r="H552">
         <v>0</v>
@@ -30174,8 +30178,8 @@
       <c r="F554">
         <v>1</v>
       </c>
-      <c r="G554" t="s">
-        <v>19</v>
+      <c r="G554">
+        <v>1</v>
       </c>
       <c r="H554">
         <v>0</v>
@@ -30284,7 +30288,7 @@
         <v>4.4720719109163267E-5</v>
       </c>
       <c r="H556">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I556" t="s">
         <v>22</v>
@@ -30333,8 +30337,8 @@
       <c r="F557">
         <v>1</v>
       </c>
-      <c r="G557" t="s">
-        <v>19</v>
+      <c r="G557">
+        <v>1</v>
       </c>
       <c r="H557">
         <v>0</v>
@@ -30492,8 +30496,8 @@
       <c r="F560">
         <v>1</v>
       </c>
-      <c r="G560" t="s">
-        <v>19</v>
+      <c r="G560">
+        <v>1</v>
       </c>
       <c r="H560">
         <v>0</v>
@@ -30651,8 +30655,8 @@
       <c r="F563">
         <v>1</v>
       </c>
-      <c r="G563" t="s">
-        <v>19</v>
+      <c r="G563">
+        <v>1</v>
       </c>
       <c r="H563">
         <v>0</v>
@@ -30757,8 +30761,8 @@
       <c r="F565">
         <v>1</v>
       </c>
-      <c r="G565" t="s">
-        <v>19</v>
+      <c r="G565">
+        <v>1</v>
       </c>
       <c r="H565">
         <v>0</v>
@@ -30810,8 +30814,8 @@
       <c r="F566">
         <v>1</v>
       </c>
-      <c r="G566" t="s">
-        <v>19</v>
+      <c r="G566">
+        <v>1</v>
       </c>
       <c r="H566">
         <v>0</v>
@@ -30863,8 +30867,8 @@
       <c r="F567">
         <v>1</v>
       </c>
-      <c r="G567" t="s">
-        <v>19</v>
+      <c r="G567">
+        <v>1</v>
       </c>
       <c r="H567">
         <v>0</v>
@@ -31075,8 +31079,8 @@
       <c r="F571">
         <v>1</v>
       </c>
-      <c r="G571" t="s">
-        <v>19</v>
+      <c r="G571">
+        <v>1</v>
       </c>
       <c r="H571">
         <v>0</v>
@@ -31234,8 +31238,8 @@
       <c r="F574">
         <v>1</v>
       </c>
-      <c r="G574" t="s">
-        <v>19</v>
+      <c r="G574">
+        <v>1</v>
       </c>
       <c r="H574">
         <v>0</v>
@@ -31287,8 +31291,8 @@
       <c r="F575">
         <v>1</v>
       </c>
-      <c r="G575" t="s">
-        <v>19</v>
+      <c r="G575">
+        <v>1</v>
       </c>
       <c r="H575">
         <v>0</v>
@@ -31499,8 +31503,8 @@
       <c r="F579">
         <v>1</v>
       </c>
-      <c r="G579" t="s">
-        <v>19</v>
+      <c r="G579">
+        <v>1</v>
       </c>
       <c r="H579">
         <v>0</v>
@@ -31605,8 +31609,8 @@
       <c r="F581">
         <v>1</v>
       </c>
-      <c r="G581" t="s">
-        <v>19</v>
+      <c r="G581">
+        <v>1</v>
       </c>
       <c r="H581">
         <v>0</v>
@@ -31817,8 +31821,8 @@
       <c r="F585">
         <v>1</v>
       </c>
-      <c r="G585" t="s">
-        <v>19</v>
+      <c r="G585">
+        <v>1</v>
       </c>
       <c r="H585">
         <v>0</v>
@@ -32029,8 +32033,8 @@
       <c r="F589">
         <v>1</v>
       </c>
-      <c r="G589" t="s">
-        <v>19</v>
+      <c r="G589">
+        <v>1</v>
       </c>
       <c r="H589">
         <v>0</v>
@@ -32082,8 +32086,8 @@
       <c r="F590">
         <v>1</v>
       </c>
-      <c r="G590" t="s">
-        <v>19</v>
+      <c r="G590">
+        <v>1</v>
       </c>
       <c r="H590">
         <v>0</v>
@@ -32192,7 +32196,7 @@
         <v>3.8649583550737241E-5</v>
       </c>
       <c r="H592">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I592" t="s">
         <v>22</v>
@@ -32241,8 +32245,8 @@
       <c r="F593">
         <v>1</v>
       </c>
-      <c r="G593" t="s">
-        <v>19</v>
+      <c r="G593">
+        <v>1</v>
       </c>
       <c r="H593">
         <v>0</v>
@@ -32400,8 +32404,8 @@
       <c r="F596">
         <v>1</v>
       </c>
-      <c r="G596" t="s">
-        <v>19</v>
+      <c r="G596">
+        <v>1</v>
       </c>
       <c r="H596">
         <v>0</v>
@@ -32559,8 +32563,8 @@
       <c r="F599">
         <v>1</v>
       </c>
-      <c r="G599" t="s">
-        <v>19</v>
+      <c r="G599">
+        <v>1</v>
       </c>
       <c r="H599">
         <v>0</v>
@@ -32665,8 +32669,8 @@
       <c r="F601">
         <v>1</v>
       </c>
-      <c r="G601" t="s">
-        <v>19</v>
+      <c r="G601">
+        <v>1</v>
       </c>
       <c r="H601">
         <v>0</v>
@@ -32718,8 +32722,8 @@
       <c r="F602">
         <v>1</v>
       </c>
-      <c r="G602" t="s">
-        <v>19</v>
+      <c r="G602">
+        <v>1</v>
       </c>
       <c r="H602">
         <v>0</v>
@@ -32771,8 +32775,8 @@
       <c r="F603">
         <v>1</v>
       </c>
-      <c r="G603" t="s">
-        <v>19</v>
+      <c r="G603">
+        <v>1</v>
       </c>
       <c r="H603">
         <v>0</v>
@@ -32987,7 +32991,7 @@
         <v>9.372071227741331E-4</v>
       </c>
       <c r="H607">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I607" t="s">
         <v>16</v>
@@ -33142,8 +33146,8 @@
       <c r="F610">
         <v>1</v>
       </c>
-      <c r="G610" t="s">
-        <v>19</v>
+      <c r="G610">
+        <v>1</v>
       </c>
       <c r="H610">
         <v>0</v>
@@ -33195,8 +33199,8 @@
       <c r="F611">
         <v>1</v>
       </c>
-      <c r="G611" t="s">
-        <v>19</v>
+      <c r="G611">
+        <v>1</v>
       </c>
       <c r="H611">
         <v>0</v>
@@ -33248,8 +33252,8 @@
       <c r="F612">
         <v>1</v>
       </c>
-      <c r="G612" t="s">
-        <v>19</v>
+      <c r="G612">
+        <v>1</v>
       </c>
       <c r="H612">
         <v>0</v>
@@ -33301,8 +33305,8 @@
       <c r="F613">
         <v>1</v>
       </c>
-      <c r="G613" t="s">
-        <v>19</v>
+      <c r="G613">
+        <v>1</v>
       </c>
       <c r="H613">
         <v>0</v>
@@ -33354,8 +33358,8 @@
       <c r="F614">
         <v>1</v>
       </c>
-      <c r="G614" t="s">
-        <v>19</v>
+      <c r="G614">
+        <v>1</v>
       </c>
       <c r="H614">
         <v>0</v>
@@ -33460,8 +33464,8 @@
       <c r="F616">
         <v>1</v>
       </c>
-      <c r="G616" t="s">
-        <v>19</v>
+      <c r="G616">
+        <v>1</v>
       </c>
       <c r="H616">
         <v>0</v>
@@ -33566,8 +33570,8 @@
       <c r="F618">
         <v>1</v>
       </c>
-      <c r="G618" t="s">
-        <v>19</v>
+      <c r="G618">
+        <v>1</v>
       </c>
       <c r="H618">
         <v>0</v>
@@ -33619,8 +33623,8 @@
       <c r="F619">
         <v>1</v>
       </c>
-      <c r="G619" t="s">
-        <v>19</v>
+      <c r="G619">
+        <v>1</v>
       </c>
       <c r="H619">
         <v>0</v>
@@ -33725,8 +33729,8 @@
       <c r="F621">
         <v>1</v>
       </c>
-      <c r="G621" t="s">
-        <v>19</v>
+      <c r="G621">
+        <v>1</v>
       </c>
       <c r="H621">
         <v>0</v>
@@ -33778,8 +33782,8 @@
       <c r="F622">
         <v>1</v>
       </c>
-      <c r="G622" t="s">
-        <v>19</v>
+      <c r="G622">
+        <v>1</v>
       </c>
       <c r="H622">
         <v>0</v>
@@ -33831,8 +33835,8 @@
       <c r="F623">
         <v>1</v>
       </c>
-      <c r="G623" t="s">
-        <v>19</v>
+      <c r="G623">
+        <v>1</v>
       </c>
       <c r="H623">
         <v>0</v>
@@ -33884,8 +33888,8 @@
       <c r="F624">
         <v>1</v>
       </c>
-      <c r="G624" t="s">
-        <v>19</v>
+      <c r="G624">
+        <v>1</v>
       </c>
       <c r="H624">
         <v>0</v>
@@ -34259,7 +34263,7 @@
         <v>3.2032181168057212E-3</v>
       </c>
       <c r="H631">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I631" t="s">
         <v>16</v>
@@ -34785,8 +34789,8 @@
       <c r="F641">
         <v>1</v>
       </c>
-      <c r="G641" t="s">
-        <v>19</v>
+      <c r="G641">
+        <v>1</v>
       </c>
       <c r="H641">
         <v>0</v>
@@ -34838,8 +34842,8 @@
       <c r="F642">
         <v>1</v>
       </c>
-      <c r="G642" t="s">
-        <v>19</v>
+      <c r="G642">
+        <v>1</v>
       </c>
       <c r="H642">
         <v>0</v>
@@ -35300,8 +35304,8 @@
       <c r="F651">
         <v>1</v>
       </c>
-      <c r="G651" t="s">
-        <v>19</v>
+      <c r="G651">
+        <v>1</v>
       </c>
       <c r="H651">
         <v>0</v>
@@ -35353,8 +35357,8 @@
       <c r="F652">
         <v>1</v>
       </c>
-      <c r="G652" t="s">
-        <v>19</v>
+      <c r="G652">
+        <v>1</v>
       </c>
       <c r="H652">
         <v>0</v>
@@ -35406,8 +35410,8 @@
       <c r="F653">
         <v>1</v>
       </c>
-      <c r="G653" t="s">
-        <v>19</v>
+      <c r="G653">
+        <v>1</v>
       </c>
       <c r="H653">
         <v>0</v>
@@ -35459,8 +35463,8 @@
       <c r="F654">
         <v>1</v>
       </c>
-      <c r="G654" t="s">
-        <v>19</v>
+      <c r="G654">
+        <v>1</v>
       </c>
       <c r="H654">
         <v>0</v>
@@ -35724,8 +35728,8 @@
       <c r="F659">
         <v>1</v>
       </c>
-      <c r="G659" t="s">
-        <v>19</v>
+      <c r="G659">
+        <v>1</v>
       </c>
       <c r="H659">
         <v>0</v>
@@ -35777,8 +35781,8 @@
       <c r="F660">
         <v>1</v>
       </c>
-      <c r="G660" t="s">
-        <v>19</v>
+      <c r="G660">
+        <v>1</v>
       </c>
       <c r="H660">
         <v>0</v>
@@ -35830,8 +35834,8 @@
       <c r="F661">
         <v>1</v>
       </c>
-      <c r="G661" t="s">
-        <v>19</v>
+      <c r="G661">
+        <v>1</v>
       </c>
       <c r="H661">
         <v>0</v>
@@ -35883,8 +35887,8 @@
       <c r="F662">
         <v>1</v>
       </c>
-      <c r="G662" t="s">
-        <v>19</v>
+      <c r="G662">
+        <v>1</v>
       </c>
       <c r="H662">
         <v>0</v>
@@ -35936,8 +35940,8 @@
       <c r="F663">
         <v>1</v>
       </c>
-      <c r="G663" t="s">
-        <v>19</v>
+      <c r="G663">
+        <v>1</v>
       </c>
       <c r="H663">
         <v>0</v>
@@ -35989,8 +35993,8 @@
       <c r="F664">
         <v>1</v>
       </c>
-      <c r="G664" t="s">
-        <v>19</v>
+      <c r="G664">
+        <v>1</v>
       </c>
       <c r="H664">
         <v>0</v>
@@ -36095,8 +36099,8 @@
       <c r="F666">
         <v>1</v>
       </c>
-      <c r="G666" t="s">
-        <v>19</v>
+      <c r="G666">
+        <v>1</v>
       </c>
       <c r="H666">
         <v>0</v>
@@ -36254,8 +36258,8 @@
       <c r="F669">
         <v>1</v>
       </c>
-      <c r="G669" t="s">
-        <v>19</v>
+      <c r="G669">
+        <v>1</v>
       </c>
       <c r="H669">
         <v>0</v>
@@ -36307,8 +36311,8 @@
       <c r="F670">
         <v>1</v>
       </c>
-      <c r="G670" t="s">
-        <v>19</v>
+      <c r="G670">
+        <v>1</v>
       </c>
       <c r="H670">
         <v>0</v>
@@ -36360,8 +36364,8 @@
       <c r="F671">
         <v>1</v>
       </c>
-      <c r="G671" t="s">
-        <v>19</v>
+      <c r="G671">
+        <v>1</v>
       </c>
       <c r="H671">
         <v>0</v>
@@ -36519,8 +36523,8 @@
       <c r="F674">
         <v>1</v>
       </c>
-      <c r="G674" t="s">
-        <v>19</v>
+      <c r="G674">
+        <v>1</v>
       </c>
       <c r="H674">
         <v>0</v>
@@ -36572,8 +36576,8 @@
       <c r="F675">
         <v>1</v>
       </c>
-      <c r="G675" t="s">
-        <v>19</v>
+      <c r="G675">
+        <v>1</v>
       </c>
       <c r="H675">
         <v>0</v>
@@ -36625,8 +36629,8 @@
       <c r="F676">
         <v>1</v>
       </c>
-      <c r="G676" t="s">
-        <v>19</v>
+      <c r="G676">
+        <v>1</v>
       </c>
       <c r="H676">
         <v>0</v>
@@ -36678,8 +36682,8 @@
       <c r="F677">
         <v>1</v>
       </c>
-      <c r="G677" t="s">
-        <v>19</v>
+      <c r="G677">
+        <v>1</v>
       </c>
       <c r="H677">
         <v>0</v>
@@ -36837,8 +36841,8 @@
       <c r="F680">
         <v>1</v>
       </c>
-      <c r="G680" t="s">
-        <v>19</v>
+      <c r="G680">
+        <v>1</v>
       </c>
       <c r="H680">
         <v>0</v>
@@ -36890,8 +36894,8 @@
       <c r="F681">
         <v>1</v>
       </c>
-      <c r="G681" t="s">
-        <v>19</v>
+      <c r="G681">
+        <v>1</v>
       </c>
       <c r="H681">
         <v>0</v>
@@ -36943,8 +36947,8 @@
       <c r="F682">
         <v>1</v>
       </c>
-      <c r="G682" t="s">
-        <v>19</v>
+      <c r="G682">
+        <v>1</v>
       </c>
       <c r="H682">
         <v>0</v>
@@ -36996,8 +37000,8 @@
       <c r="F683">
         <v>1</v>
       </c>
-      <c r="G683" t="s">
-        <v>19</v>
+      <c r="G683">
+        <v>1</v>
       </c>
       <c r="H683">
         <v>0</v>
@@ -37049,8 +37053,8 @@
       <c r="F684">
         <v>1</v>
       </c>
-      <c r="G684" t="s">
-        <v>19</v>
+      <c r="G684">
+        <v>1</v>
       </c>
       <c r="H684">
         <v>0</v>
@@ -37632,8 +37636,8 @@
       <c r="F695">
         <v>1</v>
       </c>
-      <c r="G695" t="s">
-        <v>19</v>
+      <c r="G695">
+        <v>1</v>
       </c>
       <c r="H695">
         <v>0</v>
@@ -37791,8 +37795,8 @@
       <c r="F698">
         <v>1</v>
       </c>
-      <c r="G698" t="s">
-        <v>19</v>
+      <c r="G698">
+        <v>1</v>
       </c>
       <c r="H698">
         <v>0</v>
@@ -37844,8 +37848,8 @@
       <c r="F699">
         <v>1</v>
       </c>
-      <c r="G699" t="s">
-        <v>19</v>
+      <c r="G699">
+        <v>1</v>
       </c>
       <c r="H699">
         <v>0</v>
@@ -38109,8 +38113,8 @@
       <c r="F704">
         <v>1</v>
       </c>
-      <c r="G704" t="s">
-        <v>19</v>
+      <c r="G704">
+        <v>1</v>
       </c>
       <c r="H704">
         <v>0</v>
@@ -38162,11 +38166,11 @@
       <c r="F705">
         <v>1</v>
       </c>
-      <c r="G705" t="s">
-        <v>19</v>
+      <c r="G705">
+        <v>1</v>
       </c>
       <c r="H705">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I705" t="s">
         <v>16</v>
@@ -38686,8 +38690,8 @@
       <c r="F715">
         <v>1</v>
       </c>
-      <c r="G715" t="s">
-        <v>19</v>
+      <c r="G715">
+        <v>1</v>
       </c>
       <c r="H715">
         <v>0</v>
@@ -38739,8 +38743,8 @@
       <c r="F716">
         <v>1</v>
       </c>
-      <c r="G716" t="s">
-        <v>19</v>
+      <c r="G716">
+        <v>1</v>
       </c>
       <c r="H716">
         <v>0</v>
@@ -38792,8 +38796,8 @@
       <c r="F717">
         <v>1</v>
       </c>
-      <c r="G717" t="s">
-        <v>19</v>
+      <c r="G717">
+        <v>1</v>
       </c>
       <c r="H717">
         <v>0</v>
@@ -38845,8 +38849,8 @@
       <c r="F718">
         <v>1</v>
       </c>
-      <c r="G718" t="s">
-        <v>19</v>
+      <c r="G718">
+        <v>1</v>
       </c>
       <c r="H718">
         <v>0</v>
@@ -38898,8 +38902,8 @@
       <c r="F719">
         <v>1</v>
       </c>
-      <c r="G719" t="s">
-        <v>19</v>
+      <c r="G719">
+        <v>1</v>
       </c>
       <c r="H719">
         <v>0</v>
@@ -39428,8 +39432,8 @@
       <c r="F729">
         <v>1</v>
       </c>
-      <c r="G729" t="s">
-        <v>19</v>
+      <c r="G729">
+        <v>1</v>
       </c>
       <c r="H729">
         <v>0</v>
@@ -39587,8 +39591,8 @@
       <c r="F732">
         <v>1</v>
       </c>
-      <c r="G732" t="s">
-        <v>19</v>
+      <c r="G732">
+        <v>1</v>
       </c>
       <c r="H732">
         <v>0</v>
@@ -39640,8 +39644,8 @@
       <c r="F733">
         <v>1</v>
       </c>
-      <c r="G733" t="s">
-        <v>19</v>
+      <c r="G733">
+        <v>1</v>
       </c>
       <c r="H733">
         <v>0</v>
@@ -40058,8 +40062,8 @@
       <c r="F741">
         <v>1</v>
       </c>
-      <c r="G741" t="s">
-        <v>19</v>
+      <c r="G741">
+        <v>1</v>
       </c>
       <c r="H741">
         <v>0</v>
@@ -40111,11 +40115,11 @@
       <c r="F742">
         <v>1</v>
       </c>
-      <c r="G742" t="s">
-        <v>19</v>
+      <c r="G742">
+        <v>1</v>
       </c>
       <c r="H742">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I742" t="s">
         <v>16</v>
@@ -40270,8 +40274,8 @@
       <c r="F745">
         <v>1</v>
       </c>
-      <c r="G745" t="s">
-        <v>19</v>
+      <c r="G745">
+        <v>1</v>
       </c>
       <c r="H745">
         <v>0</v>
@@ -40323,8 +40327,8 @@
       <c r="F746">
         <v>1</v>
       </c>
-      <c r="G746" t="s">
-        <v>19</v>
+      <c r="G746">
+        <v>1</v>
       </c>
       <c r="H746">
         <v>0</v>
@@ -40376,8 +40380,8 @@
       <c r="F747">
         <v>1</v>
       </c>
-      <c r="G747" t="s">
-        <v>19</v>
+      <c r="G747">
+        <v>1</v>
       </c>
       <c r="H747">
         <v>0</v>
@@ -40429,8 +40433,8 @@
       <c r="F748">
         <v>1</v>
       </c>
-      <c r="G748" t="s">
-        <v>19</v>
+      <c r="G748">
+        <v>1</v>
       </c>
       <c r="H748">
         <v>0</v>
@@ -40482,8 +40486,8 @@
       <c r="F749">
         <v>1</v>
       </c>
-      <c r="G749" t="s">
-        <v>19</v>
+      <c r="G749">
+        <v>1</v>
       </c>
       <c r="H749">
         <v>0</v>
@@ -40535,8 +40539,8 @@
       <c r="F750">
         <v>1</v>
       </c>
-      <c r="G750" t="s">
-        <v>19</v>
+      <c r="G750">
+        <v>1</v>
       </c>
       <c r="H750">
         <v>0</v>
@@ -40588,8 +40592,8 @@
       <c r="F751">
         <v>1</v>
       </c>
-      <c r="G751" t="s">
-        <v>19</v>
+      <c r="G751">
+        <v>1</v>
       </c>
       <c r="H751">
         <v>0</v>
@@ -40853,8 +40857,8 @@
       <c r="F756">
         <v>1</v>
       </c>
-      <c r="G756" t="s">
-        <v>19</v>
+      <c r="G756">
+        <v>1</v>
       </c>
       <c r="H756">
         <v>0</v>
@@ -40906,8 +40910,8 @@
       <c r="F757">
         <v>1</v>
       </c>
-      <c r="G757" t="s">
-        <v>19</v>
+      <c r="G757">
+        <v>1</v>
       </c>
       <c r="H757">
         <v>0</v>
@@ -40959,8 +40963,8 @@
       <c r="F758">
         <v>1</v>
       </c>
-      <c r="G758" t="s">
-        <v>19</v>
+      <c r="G758">
+        <v>1</v>
       </c>
       <c r="H758">
         <v>0</v>
@@ -41012,8 +41016,8 @@
       <c r="F759">
         <v>1</v>
       </c>
-      <c r="G759" t="s">
-        <v>19</v>
+      <c r="G759">
+        <v>1</v>
       </c>
       <c r="H759">
         <v>0</v>
@@ -41065,8 +41069,8 @@
       <c r="F760">
         <v>1</v>
       </c>
-      <c r="G760" t="s">
-        <v>19</v>
+      <c r="G760">
+        <v>1</v>
       </c>
       <c r="H760">
         <v>0</v>
@@ -41118,8 +41122,8 @@
       <c r="F761">
         <v>1</v>
       </c>
-      <c r="G761" t="s">
-        <v>19</v>
+      <c r="G761">
+        <v>1</v>
       </c>
       <c r="H761">
         <v>0</v>
@@ -41224,8 +41228,8 @@
       <c r="F763">
         <v>1</v>
       </c>
-      <c r="G763" t="s">
-        <v>19</v>
+      <c r="G763">
+        <v>1</v>
       </c>
       <c r="H763">
         <v>0</v>
@@ -41383,8 +41387,8 @@
       <c r="F766">
         <v>1</v>
       </c>
-      <c r="G766" t="s">
-        <v>19</v>
+      <c r="G766">
+        <v>1</v>
       </c>
       <c r="H766">
         <v>0</v>
@@ -41436,8 +41440,8 @@
       <c r="F767">
         <v>1</v>
       </c>
-      <c r="G767" t="s">
-        <v>19</v>
+      <c r="G767">
+        <v>1</v>
       </c>
       <c r="H767">
         <v>0</v>
@@ -41489,8 +41493,8 @@
       <c r="F768">
         <v>1</v>
       </c>
-      <c r="G768" t="s">
-        <v>19</v>
+      <c r="G768">
+        <v>1</v>
       </c>
       <c r="H768">
         <v>0</v>
@@ -41648,8 +41652,8 @@
       <c r="F771">
         <v>1</v>
       </c>
-      <c r="G771" t="s">
-        <v>19</v>
+      <c r="G771">
+        <v>1</v>
       </c>
       <c r="H771">
         <v>0</v>
@@ -41701,8 +41705,8 @@
       <c r="F772">
         <v>1</v>
       </c>
-      <c r="G772" t="s">
-        <v>19</v>
+      <c r="G772">
+        <v>1</v>
       </c>
       <c r="H772">
         <v>0</v>
@@ -41754,8 +41758,8 @@
       <c r="F773">
         <v>1</v>
       </c>
-      <c r="G773" t="s">
-        <v>19</v>
+      <c r="G773">
+        <v>1</v>
       </c>
       <c r="H773">
         <v>0</v>
@@ -41807,8 +41811,8 @@
       <c r="F774">
         <v>1</v>
       </c>
-      <c r="G774" t="s">
-        <v>19</v>
+      <c r="G774">
+        <v>1</v>
       </c>
       <c r="H774">
         <v>0</v>
@@ -42178,8 +42182,8 @@
       <c r="F781">
         <v>1</v>
       </c>
-      <c r="G781" t="s">
-        <v>19</v>
+      <c r="G781">
+        <v>1</v>
       </c>
       <c r="H781">
         <v>0</v>
@@ -42231,8 +42235,8 @@
       <c r="F782">
         <v>1</v>
       </c>
-      <c r="G782" t="s">
-        <v>19</v>
+      <c r="G782">
+        <v>1</v>
       </c>
       <c r="H782">
         <v>0</v>
@@ -42284,8 +42288,8 @@
       <c r="F783">
         <v>1</v>
       </c>
-      <c r="G783" t="s">
-        <v>19</v>
+      <c r="G783">
+        <v>1</v>
       </c>
       <c r="H783">
         <v>0</v>
@@ -42337,8 +42341,8 @@
       <c r="F784">
         <v>1</v>
       </c>
-      <c r="G784" t="s">
-        <v>19</v>
+      <c r="G784">
+        <v>1</v>
       </c>
       <c r="H784">
         <v>0</v>
@@ -42390,8 +42394,8 @@
       <c r="F785">
         <v>1</v>
       </c>
-      <c r="G785" t="s">
-        <v>19</v>
+      <c r="G785">
+        <v>1</v>
       </c>
       <c r="H785">
         <v>0</v>
@@ -42443,8 +42447,8 @@
       <c r="F786">
         <v>1</v>
       </c>
-      <c r="G786" t="s">
-        <v>19</v>
+      <c r="G786">
+        <v>1</v>
       </c>
       <c r="H786">
         <v>0</v>
@@ -42549,8 +42553,8 @@
       <c r="F788">
         <v>1</v>
       </c>
-      <c r="G788" t="s">
-        <v>19</v>
+      <c r="G788">
+        <v>1</v>
       </c>
       <c r="H788">
         <v>0</v>
@@ -42708,8 +42712,8 @@
       <c r="F791">
         <v>1</v>
       </c>
-      <c r="G791" t="s">
-        <v>19</v>
+      <c r="G791">
+        <v>1</v>
       </c>
       <c r="H791">
         <v>0</v>
@@ -42761,8 +42765,8 @@
       <c r="F792">
         <v>1</v>
       </c>
-      <c r="G792" t="s">
-        <v>19</v>
+      <c r="G792">
+        <v>1</v>
       </c>
       <c r="H792">
         <v>0</v>
@@ -42814,8 +42818,8 @@
       <c r="F793">
         <v>1</v>
       </c>
-      <c r="G793" t="s">
-        <v>19</v>
+      <c r="G793">
+        <v>1</v>
       </c>
       <c r="H793">
         <v>0</v>
@@ -42973,8 +42977,8 @@
       <c r="F796">
         <v>1</v>
       </c>
-      <c r="G796" t="s">
-        <v>19</v>
+      <c r="G796">
+        <v>1</v>
       </c>
       <c r="H796">
         <v>0</v>
@@ -43026,8 +43030,8 @@
       <c r="F797">
         <v>1</v>
       </c>
-      <c r="G797" t="s">
-        <v>19</v>
+      <c r="G797">
+        <v>1</v>
       </c>
       <c r="H797">
         <v>0</v>
@@ -43079,8 +43083,8 @@
       <c r="F798">
         <v>1</v>
       </c>
-      <c r="G798" t="s">
-        <v>19</v>
+      <c r="G798">
+        <v>1</v>
       </c>
       <c r="H798">
         <v>0</v>
@@ -43132,8 +43136,8 @@
       <c r="F799">
         <v>1</v>
       </c>
-      <c r="G799" t="s">
-        <v>19</v>
+      <c r="G799">
+        <v>1</v>
       </c>
       <c r="H799">
         <v>0</v>
@@ -43291,8 +43295,8 @@
       <c r="F802">
         <v>1</v>
       </c>
-      <c r="G802" t="s">
-        <v>19</v>
+      <c r="G802">
+        <v>1</v>
       </c>
       <c r="H802">
         <v>0</v>
@@ -43344,8 +43348,8 @@
       <c r="F803">
         <v>1</v>
       </c>
-      <c r="G803" t="s">
-        <v>19</v>
+      <c r="G803">
+        <v>1</v>
       </c>
       <c r="H803">
         <v>0</v>
@@ -43397,8 +43401,8 @@
       <c r="F804">
         <v>1</v>
       </c>
-      <c r="G804" t="s">
-        <v>19</v>
+      <c r="G804">
+        <v>1</v>
       </c>
       <c r="H804">
         <v>0</v>

</xml_diff>